<commit_message>
Add new figure for stream width estimation
</commit_message>
<xml_diff>
--- a/data/Navarro_StreamWidthEstimates.xlsx
+++ b/data/Navarro_StreamWidthEstimates.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\WorkGits\TNC-PilotProject\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4598737-6BAE-44CB-B515-88CEAEAE30D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8808"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -77,7 +78,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -136,7 +137,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -150,7 +151,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -411,6 +411,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-63CB-47E7-8B41-FA96F30B39C4}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -456,7 +461,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -560,7 +564,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1249,7 +1252,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1529,27 +1538,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1566,7 +1575,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>61</v>
       </c>
@@ -1583,7 +1592,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>70</v>
       </c>
@@ -1600,7 +1609,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>68</v>
       </c>
@@ -1617,7 +1626,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>73</v>
       </c>
@@ -1634,7 +1643,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>83</v>
       </c>
@@ -1651,7 +1660,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>85</v>
       </c>
@@ -1668,7 +1677,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>102</v>
       </c>
@@ -1682,7 +1691,7 @@
         <v>15.7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>330</v>
       </c>
@@ -1696,7 +1705,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>237</v>
       </c>
@@ -1713,7 +1722,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>240</v>
       </c>
@@ -1730,7 +1739,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>257</v>
       </c>
@@ -1744,7 +1753,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>119</v>
       </c>
@@ -1758,7 +1767,7 @@
         <v>22.43</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>66</v>
       </c>
@@ -1772,7 +1781,7 @@
         <v>24.74</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>92</v>
       </c>
@@ -1786,7 +1795,7 @@
         <v>24.63</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>74</v>
       </c>
@@ -1803,7 +1812,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>73</v>
       </c>
@@ -1817,7 +1826,7 @@
         <v>45.54</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>228</v>
       </c>
@@ -1831,7 +1840,7 @@
         <v>19.95</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>84</v>
       </c>
@@ -1845,7 +1854,7 @@
         <v>22.2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>62</v>
       </c>
@@ -1862,7 +1871,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>63</v>
       </c>

</xml_diff>